<commit_message>
FACET vectors generated for 339-377 videos
</commit_message>
<xml_diff>
--- a/data/QuestionsClassification.xlsx
+++ b/data/QuestionsClassification.xlsx
@@ -1,19 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Madhusudhan/Fall 2016/CSCI 535/Project/Depression-Identification/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="240" yWindow="440" windowWidth="25360" windowHeight="14440" tabRatio="500" activeTab="1"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet3" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Annotation-Supervised" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="Annotations-Unsupervised" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="1" r:id="rId1"/>
+    <sheet name="Annotation-Supervised" sheetId="2" r:id="rId2"/>
+    <sheet name="Annotations-Unsupervised" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="79">
   <si>
     <t>Questions</t>
   </si>
@@ -247,33 +263,41 @@
   </si>
   <si>
     <t>what are some things you like to do for fun who's someone that's been a positive influence in your life</t>
+  </si>
+  <si>
+    <t xml:space="preserve">how close are you to your family </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -288,98 +312,333 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="83.57"/>
-    <col customWidth="1" min="2" max="2" width="38.57"/>
-    <col customWidth="1" min="3" max="3" width="45.0"/>
-    <col hidden="1" min="6" max="6"/>
-    <col customWidth="1" min="10" max="10" width="12.43"/>
+    <col min="1" max="1" width="83.5" customWidth="1"/>
+    <col min="2" max="2" width="38.5" customWidth="1"/>
+    <col min="3" max="3" width="45" customWidth="1"/>
+    <col min="6" max="6" width="0" hidden="1"/>
+    <col min="10" max="10" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -399,7 +658,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
@@ -416,7 +675,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
@@ -436,7 +695,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="12" t="s">
         <v>15</v>
       </c>
@@ -456,7 +715,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="12" t="s">
         <v>21</v>
       </c>
@@ -476,7 +735,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>24</v>
       </c>
@@ -496,7 +755,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
         <v>25</v>
       </c>
@@ -516,7 +775,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>28</v>
       </c>
@@ -530,7 +789,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
         <v>29</v>
       </c>
@@ -550,7 +809,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
         <v>32</v>
       </c>
@@ -570,7 +829,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
         <v>34</v>
       </c>
@@ -590,7 +849,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="12" t="s">
         <v>36</v>
       </c>
@@ -610,7 +869,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
         <v>39</v>
       </c>
@@ -630,7 +889,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
         <v>40</v>
       </c>
@@ -650,7 +909,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="7" t="s">
         <v>41</v>
       </c>
@@ -670,7 +929,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="7" t="s">
         <v>42</v>
       </c>
@@ -690,7 +949,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="12" t="s">
         <v>44</v>
       </c>
@@ -710,7 +969,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
         <v>48</v>
       </c>
@@ -730,7 +989,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="12" t="s">
         <v>49</v>
       </c>
@@ -750,7 +1009,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="7" t="s">
         <v>52</v>
       </c>
@@ -770,7 +1029,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
         <v>54</v>
       </c>
@@ -790,7 +1049,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="7" t="s">
         <v>55</v>
       </c>
@@ -810,7 +1069,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="12" t="s">
         <v>56</v>
       </c>
@@ -830,7 +1089,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
         <v>59</v>
       </c>
@@ -850,7 +1109,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -870,7 +1129,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="7" t="s">
         <v>62</v>
       </c>
@@ -890,7 +1149,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="7" t="s">
         <v>64</v>
       </c>
@@ -910,7 +1169,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="7" t="s">
         <v>67</v>
       </c>
@@ -930,7 +1189,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="12" t="s">
         <v>69</v>
       </c>
@@ -950,7 +1209,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="7" t="s">
         <v>72</v>
       </c>
@@ -971,21 +1230,24 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y138"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="68.71"/>
+    <col min="1" max="1" width="68.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -998,7 +1260,7 @@
       <c r="F1" s="8"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="s">
         <v>8</v>
       </c>
@@ -1010,7 +1272,7 @@
       <c r="H2" s="10"/>
       <c r="J2" s="11"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
         <v>17</v>
       </c>
@@ -1025,7 +1287,7 @@
       <c r="I3" s="7"/>
       <c r="J3" s="11"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -1040,7 +1302,7 @@
       <c r="I4" s="7"/>
       <c r="J4" s="11"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
@@ -1055,7 +1317,7 @@
       <c r="I5" s="7"/>
       <c r="J5" s="11"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1068,7 +1330,7 @@
       <c r="F6" s="8"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="13" t="s">
         <v>15</v>
       </c>
@@ -1081,7 +1343,7 @@
       <c r="F7" s="10"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
         <v>15</v>
       </c>
@@ -1092,7 +1354,7 @@
       <c r="F8" s="10"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
         <v>15</v>
       </c>
@@ -1104,7 +1366,7 @@
       <c r="F9" s="10"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
         <v>21</v>
       </c>
@@ -1115,7 +1377,7 @@
       <c r="F10" s="10"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="13" t="s">
         <v>21</v>
       </c>
@@ -1128,7 +1390,7 @@
       <c r="F11" s="10"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -1141,7 +1403,7 @@
       <c r="F12" s="10"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
         <v>24</v>
       </c>
@@ -1152,7 +1414,7 @@
       <c r="F13" s="8"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="s">
         <v>24</v>
       </c>
@@ -1165,7 +1427,7 @@
       <c r="F14" s="8"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
@@ -1178,7 +1440,7 @@
       <c r="F15" s="8"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="s">
         <v>25</v>
       </c>
@@ -1189,7 +1451,7 @@
       <c r="F16" s="8"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13" t="s">
         <v>25</v>
       </c>
@@ -1202,7 +1464,7 @@
       <c r="F17" s="8"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="s">
         <v>25</v>
       </c>
@@ -1215,7 +1477,7 @@
       <c r="F18" s="8"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>28</v>
       </c>
@@ -1226,7 +1488,7 @@
       <c r="F19" s="10"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="s">
         <v>28</v>
       </c>
@@ -1239,9 +1501,9 @@
       <c r="F20" s="10"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>23</v>
@@ -1252,7 +1514,7 @@
       <c r="F21" s="10"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="12" t="s">
         <v>29</v>
       </c>
@@ -1263,7 +1525,7 @@
       <c r="F22" s="10"/>
       <c r="H22" s="10"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="13" t="s">
         <v>29</v>
       </c>
@@ -1278,7 +1540,7 @@
       <c r="H23" s="10"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="s">
         <v>29</v>
       </c>
@@ -1293,7 +1555,7 @@
       <c r="H24" s="10"/>
       <c r="I24" s="7"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="7" t="s">
         <v>38</v>
       </c>
@@ -1308,7 +1570,7 @@
       <c r="H25" s="10"/>
       <c r="I25" s="7"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="7" t="s">
         <v>29</v>
       </c>
@@ -1323,7 +1585,7 @@
       <c r="H26" s="10"/>
       <c r="I26" s="7"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="7" t="s">
         <v>32</v>
       </c>
@@ -1334,7 +1596,7 @@
       <c r="F27" s="8"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
         <v>32</v>
       </c>
@@ -1347,7 +1609,7 @@
       <c r="F28" s="8"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="s">
         <v>32</v>
       </c>
@@ -1360,7 +1622,7 @@
       <c r="F29" s="8"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="12" t="s">
         <v>34</v>
       </c>
@@ -1371,7 +1633,7 @@
       <c r="F30" s="10"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="13" t="s">
         <v>34</v>
       </c>
@@ -1385,7 +1647,7 @@
       <c r="G31" s="7"/>
       <c r="H31" s="5"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="9" t="s">
         <v>47</v>
       </c>
@@ -1399,7 +1661,7 @@
       <c r="G32" s="7"/>
       <c r="H32" s="5"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="7" t="s">
         <v>34</v>
       </c>
@@ -1413,7 +1675,7 @@
       <c r="G33" s="7"/>
       <c r="H33" s="5"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="12" t="s">
         <v>36</v>
       </c>
@@ -1424,7 +1686,7 @@
       <c r="F34" s="10"/>
       <c r="H34" s="5"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="13" t="s">
         <v>36</v>
       </c>
@@ -1438,7 +1700,7 @@
       <c r="G35" s="7"/>
       <c r="H35" s="5"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="s">
         <v>53</v>
       </c>
@@ -1452,7 +1714,7 @@
       <c r="G36" s="7"/>
       <c r="H36" s="5"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="7" t="s">
         <v>36</v>
       </c>
@@ -1466,7 +1728,7 @@
       <c r="G37" s="7"/>
       <c r="H37" s="5"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="7" t="s">
         <v>39</v>
       </c>
@@ -1478,7 +1740,7 @@
       <c r="F38" s="8"/>
       <c r="H38" s="5"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="5" t="s">
         <v>39</v>
       </c>
@@ -1491,7 +1753,7 @@
       <c r="F39" s="8"/>
       <c r="H39" s="5"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="7" t="s">
         <v>40</v>
       </c>
@@ -1503,7 +1765,7 @@
       <c r="F40" s="8"/>
       <c r="H40" s="5"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A41" s="5" t="s">
         <v>40</v>
       </c>
@@ -1516,7 +1778,7 @@
       <c r="F41" s="8"/>
       <c r="H41" s="5"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A42" s="7" t="s">
         <v>41</v>
       </c>
@@ -1527,7 +1789,7 @@
       <c r="F42" s="8"/>
       <c r="H42" s="5"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A43" s="9" t="s">
         <v>41</v>
       </c>
@@ -1540,7 +1802,7 @@
       <c r="F43" s="8"/>
       <c r="H43" s="5"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A44" s="9" t="s">
         <v>41</v>
       </c>
@@ -1553,7 +1815,7 @@
       <c r="F44" s="8"/>
       <c r="H44" s="5"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A45" s="7" t="s">
         <v>42</v>
       </c>
@@ -1565,7 +1827,7 @@
       <c r="F45" s="8"/>
       <c r="H45" s="5"/>
     </row>
-    <row r="46">
+    <row r="46" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A46" s="5" t="s">
         <v>42</v>
       </c>
@@ -1578,7 +1840,7 @@
       <c r="F46" s="8"/>
       <c r="H46" s="5"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A47" s="12" t="s">
         <v>44</v>
       </c>
@@ -1589,7 +1851,7 @@
       <c r="F47" s="10"/>
       <c r="H47" s="10"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A48" s="13" t="s">
         <v>44</v>
       </c>
@@ -1604,7 +1866,7 @@
       <c r="H48" s="10"/>
       <c r="I48" s="7"/>
     </row>
-    <row r="49">
+    <row r="49" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="9" t="s">
         <v>68</v>
       </c>
@@ -1619,7 +1881,7 @@
       <c r="H49" s="10"/>
       <c r="I49" s="7"/>
     </row>
-    <row r="50">
+    <row r="50" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="7" t="s">
         <v>68</v>
       </c>
@@ -1634,7 +1896,7 @@
       <c r="H50" s="10"/>
       <c r="I50" s="7"/>
     </row>
-    <row r="51">
+    <row r="51" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="7" t="s">
         <v>68</v>
       </c>
@@ -1649,7 +1911,7 @@
       <c r="H51" s="10"/>
       <c r="I51" s="7"/>
     </row>
-    <row r="52">
+    <row r="52" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="7" t="s">
         <v>48</v>
       </c>
@@ -1661,8 +1923,8 @@
       <c r="F52" s="8"/>
       <c r="H52" s="5"/>
     </row>
-    <row r="53">
-      <c r="A53" s="5" t="s">
+    <row r="53" spans="1:9" ht="13" x14ac:dyDescent="0.15">
+      <c r="A53" s="9" t="s">
         <v>48</v>
       </c>
       <c r="B53" s="5" t="s">
@@ -1674,7 +1936,7 @@
       <c r="F53" s="8"/>
       <c r="H53" s="5"/>
     </row>
-    <row r="54">
+    <row r="54" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="12" t="s">
         <v>49</v>
       </c>
@@ -1685,7 +1947,7 @@
       <c r="F54" s="10"/>
       <c r="H54" s="10"/>
     </row>
-    <row r="55">
+    <row r="55" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="13" t="s">
         <v>49</v>
       </c>
@@ -1700,7 +1962,7 @@
       <c r="H55" s="10"/>
       <c r="I55" s="7"/>
     </row>
-    <row r="56">
+    <row r="56" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="9" t="s">
         <v>73</v>
       </c>
@@ -1715,7 +1977,7 @@
       <c r="H56" s="10"/>
       <c r="I56" s="7"/>
     </row>
-    <row r="57">
+    <row r="57" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="7" t="s">
         <v>73</v>
       </c>
@@ -1730,7 +1992,7 @@
       <c r="H57" s="10"/>
       <c r="I57" s="7"/>
     </row>
-    <row r="58">
+    <row r="58" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="7" t="s">
         <v>73</v>
       </c>
@@ -1745,7 +2007,7 @@
       <c r="H58" s="10"/>
       <c r="I58" s="7"/>
     </row>
-    <row r="59">
+    <row r="59" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="7" t="s">
         <v>52</v>
       </c>
@@ -1756,7 +2018,7 @@
       <c r="F59" s="10"/>
       <c r="H59" s="5"/>
     </row>
-    <row r="60">
+    <row r="60" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="9" t="s">
         <v>52</v>
       </c>
@@ -1770,7 +2032,7 @@
       <c r="G60" s="7"/>
       <c r="H60" s="5"/>
     </row>
-    <row r="61">
+    <row r="61" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="9" t="s">
         <v>52</v>
       </c>
@@ -1784,7 +2046,7 @@
       <c r="G61" s="7"/>
       <c r="H61" s="5"/>
     </row>
-    <row r="62">
+    <row r="62" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="7" t="s">
         <v>52</v>
       </c>
@@ -1798,7 +2060,7 @@
       <c r="G62" s="7"/>
       <c r="H62" s="5"/>
     </row>
-    <row r="63">
+    <row r="63" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="5" t="s">
         <v>54</v>
       </c>
@@ -1810,7 +2072,7 @@
       <c r="F63" s="8"/>
       <c r="H63" s="5"/>
     </row>
-    <row r="64">
+    <row r="64" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="9" t="s">
         <v>55</v>
       </c>
@@ -1821,7 +2083,7 @@
       <c r="F64" s="8"/>
       <c r="H64" s="5"/>
     </row>
-    <row r="65">
+    <row r="65" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A65" s="9" t="s">
         <v>55</v>
       </c>
@@ -1834,7 +2096,7 @@
       <c r="F65" s="8"/>
       <c r="H65" s="5"/>
     </row>
-    <row r="66">
+    <row r="66" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="13" t="s">
         <v>56</v>
       </c>
@@ -1845,7 +2107,7 @@
       <c r="F66" s="8"/>
       <c r="H66" s="5"/>
     </row>
-    <row r="67">
+    <row r="67" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="9" t="s">
         <v>56</v>
       </c>
@@ -1858,7 +2120,7 @@
       <c r="F67" s="8"/>
       <c r="H67" s="5"/>
     </row>
-    <row r="68">
+    <row r="68" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="9" t="s">
         <v>59</v>
       </c>
@@ -1869,7 +2131,7 @@
       <c r="F68" s="10"/>
       <c r="H68" s="10"/>
     </row>
-    <row r="69">
+    <row r="69" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="9" t="s">
         <v>74</v>
       </c>
@@ -1884,7 +2146,7 @@
       <c r="H69" s="10"/>
       <c r="I69" s="7"/>
     </row>
-    <row r="70">
+    <row r="70" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="7" t="s">
         <v>59</v>
       </c>
@@ -1899,7 +2161,7 @@
       <c r="H70" s="10"/>
       <c r="I70" s="7"/>
     </row>
-    <row r="71">
+    <row r="71" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="7" t="s">
         <v>59</v>
       </c>
@@ -1914,7 +2176,7 @@
       <c r="H71" s="10"/>
       <c r="I71" s="7"/>
     </row>
-    <row r="72">
+    <row r="72" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="9" t="s">
         <v>61</v>
       </c>
@@ -1925,7 +2187,7 @@
       <c r="F72" s="8"/>
       <c r="H72" s="5"/>
     </row>
-    <row r="73">
+    <row r="73" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="9" t="s">
         <v>61</v>
       </c>
@@ -1938,7 +2200,7 @@
       <c r="F73" s="8"/>
       <c r="H73" s="5"/>
     </row>
-    <row r="74">
+    <row r="74" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="9" t="s">
         <v>62</v>
       </c>
@@ -1949,7 +2211,7 @@
       <c r="F74" s="8"/>
       <c r="H74" s="5"/>
     </row>
-    <row r="75">
+    <row r="75" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="9" t="s">
         <v>62</v>
       </c>
@@ -1962,7 +2224,7 @@
       <c r="F75" s="8"/>
       <c r="H75" s="5"/>
     </row>
-    <row r="76">
+    <row r="76" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="5" t="s">
         <v>64</v>
       </c>
@@ -1974,7 +2236,7 @@
       <c r="F76" s="8"/>
       <c r="H76" s="5"/>
     </row>
-    <row r="77">
+    <row r="77" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="9" t="s">
         <v>67</v>
       </c>
@@ -1985,7 +2247,7 @@
       <c r="F77" s="10"/>
       <c r="H77" s="5"/>
     </row>
-    <row r="78">
+    <row r="78" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A78" s="9" t="s">
         <v>75</v>
       </c>
@@ -1999,7 +2261,7 @@
       <c r="G78" s="7"/>
       <c r="H78" s="5"/>
     </row>
-    <row r="79">
+    <row r="79" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A79" s="7" t="s">
         <v>67</v>
       </c>
@@ -2013,7 +2275,7 @@
       <c r="G79" s="7"/>
       <c r="H79" s="5"/>
     </row>
-    <row r="80">
+    <row r="80" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A80" s="13" t="s">
         <v>69</v>
       </c>
@@ -2024,7 +2286,7 @@
       <c r="F80" s="10"/>
       <c r="H80" s="10"/>
     </row>
-    <row r="81">
+    <row r="81" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="9" t="s">
         <v>69</v>
       </c>
@@ -2039,7 +2301,7 @@
       <c r="H81" s="10"/>
       <c r="I81" s="7"/>
     </row>
-    <row r="82">
+    <row r="82" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A82" s="7" t="s">
         <v>69</v>
       </c>
@@ -2054,7 +2316,7 @@
       <c r="H82" s="10"/>
       <c r="I82" s="7"/>
     </row>
-    <row r="83">
+    <row r="83" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A83" s="7" t="s">
         <v>69</v>
       </c>
@@ -2069,7 +2331,7 @@
       <c r="H83" s="10"/>
       <c r="I83" s="7"/>
     </row>
-    <row r="84">
+    <row r="84" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A84" s="9" t="s">
         <v>72</v>
       </c>
@@ -2081,7 +2343,7 @@
       <c r="H84" s="10"/>
       <c r="J84" s="11"/>
     </row>
-    <row r="85">
+    <row r="85" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A85" s="9" t="s">
         <v>72</v>
       </c>
@@ -2089,7 +2351,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A86" s="7" t="s">
         <v>76</v>
       </c>
@@ -2097,7 +2359,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A87" s="7" t="s">
         <v>72</v>
       </c>
@@ -2105,7 +2367,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A88" s="7" t="s">
         <v>77</v>
       </c>
@@ -2113,7 +2375,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A103" s="15"/>
       <c r="C103" s="7"/>
       <c r="D103" s="16"/>
@@ -2139,137 +2401,138 @@
       <c r="X103" s="7"/>
       <c r="Y103" s="7"/>
     </row>
-    <row r="104">
+    <row r="104" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A104" s="7"/>
       <c r="D104" s="8"/>
       <c r="E104" s="5"/>
       <c r="F104" s="8"/>
       <c r="H104" s="5"/>
     </row>
-    <row r="105">
+    <row r="105" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A105" s="7"/>
       <c r="D105" s="8"/>
       <c r="E105" s="5"/>
       <c r="F105" s="8"/>
       <c r="H105" s="5"/>
     </row>
-    <row r="106">
+    <row r="106" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A106" s="7"/>
       <c r="D106" s="8"/>
       <c r="E106" s="5"/>
       <c r="F106" s="8"/>
       <c r="H106" s="5"/>
     </row>
-    <row r="107">
+    <row r="107" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A107" s="7"/>
       <c r="E107" s="5"/>
       <c r="F107" s="8"/>
       <c r="H107" s="5"/>
     </row>
-    <row r="110">
+    <row r="110" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A110" s="12"/>
     </row>
-    <row r="111">
+    <row r="111" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A111" s="12"/>
     </row>
-    <row r="112">
+    <row r="112" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A112" s="12"/>
     </row>
-    <row r="113">
+    <row r="113" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A113" s="12"/>
     </row>
-    <row r="114">
+    <row r="114" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A114" s="12"/>
     </row>
-    <row r="115">
+    <row r="115" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A115" s="12"/>
     </row>
-    <row r="116">
+    <row r="116" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A116" s="12"/>
     </row>
-    <row r="117">
+    <row r="117" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A117" s="12"/>
     </row>
-    <row r="118">
+    <row r="118" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A118" s="12"/>
     </row>
-    <row r="119">
+    <row r="119" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A119" s="12"/>
     </row>
-    <row r="120">
+    <row r="120" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A120" s="3"/>
     </row>
-    <row r="121">
+    <row r="121" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A121" s="7"/>
     </row>
-    <row r="122">
+    <row r="122" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A122" s="7"/>
     </row>
-    <row r="123">
+    <row r="123" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A123" s="7"/>
     </row>
-    <row r="124">
+    <row r="124" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A124" s="7"/>
     </row>
-    <row r="125">
+    <row r="125" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A125" s="7"/>
     </row>
-    <row r="126">
+    <row r="126" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A126" s="7"/>
     </row>
-    <row r="127">
+    <row r="127" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A127" s="7"/>
     </row>
-    <row r="128">
+    <row r="128" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A128" s="7"/>
     </row>
-    <row r="129">
+    <row r="129" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A129" s="7"/>
     </row>
-    <row r="130">
+    <row r="130" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A130" s="7"/>
     </row>
-    <row r="131">
+    <row r="131" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A131" s="7"/>
     </row>
-    <row r="132">
+    <row r="132" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A132" s="7"/>
     </row>
-    <row r="133">
+    <row r="133" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A133" s="7"/>
     </row>
-    <row r="134">
+    <row r="134" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A134" s="7"/>
     </row>
-    <row r="135">
+    <row r="135" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A135" s="7"/>
     </row>
-    <row r="136">
+    <row r="136" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A136" s="7"/>
     </row>
-    <row r="137">
+    <row r="137" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A137" s="7"/>
     </row>
-    <row r="138">
+    <row r="138" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A138" s="7"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="47.86"/>
-    <col customWidth="1" min="3" max="3" width="51.57"/>
+    <col min="1" max="1" width="47.83203125" customWidth="1"/>
+    <col min="3" max="3" width="51.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2279,7 +2542,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="s">
         <v>8</v>
       </c>
@@ -2289,7 +2552,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="8"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
         <v>17</v>
       </c>
@@ -2299,7 +2562,7 @@
       <c r="C3" s="5"/>
       <c r="D3" s="8"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -2309,7 +2572,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="8"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
@@ -2319,7 +2582,7 @@
       <c r="C5" s="5"/>
       <c r="D5" s="8"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -2329,7 +2592,7 @@
       <c r="C6" s="5"/>
       <c r="D6" s="8"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="13" t="s">
         <v>15</v>
       </c>
@@ -2339,7 +2602,7 @@
       <c r="C7" s="5"/>
       <c r="D7" s="8"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
         <v>15</v>
       </c>
@@ -2349,7 +2612,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
         <v>15</v>
       </c>
@@ -2359,7 +2622,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
         <v>21</v>
       </c>
@@ -2369,7 +2632,7 @@
       <c r="C10" s="5"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="13" t="s">
         <v>21</v>
       </c>
@@ -2379,7 +2642,7 @@
       <c r="C11" s="5"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -2389,7 +2652,7 @@
       <c r="C12" s="5"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
         <v>24</v>
       </c>
@@ -2399,7 +2662,7 @@
       <c r="C13" s="5"/>
       <c r="D13" s="8"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="s">
         <v>24</v>
       </c>
@@ -2409,7 +2672,7 @@
       <c r="C14" s="5"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
@@ -2419,7 +2682,7 @@
       <c r="C15" s="5"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="s">
         <v>25</v>
       </c>
@@ -2429,7 +2692,7 @@
       <c r="C16" s="5"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13" t="s">
         <v>25</v>
       </c>
@@ -2439,7 +2702,7 @@
       <c r="C17" s="5"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="s">
         <v>25</v>
       </c>
@@ -2449,7 +2712,7 @@
       <c r="C18" s="5"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>28</v>
       </c>
@@ -2459,7 +2722,7 @@
       <c r="C19" s="5"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="s">
         <v>28</v>
       </c>
@@ -2469,7 +2732,7 @@
       <c r="C20" s="5"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="s">
         <v>28</v>
       </c>
@@ -2479,7 +2742,7 @@
       <c r="C21" s="5"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="12" t="s">
         <v>29</v>
       </c>
@@ -2489,7 +2752,7 @@
       <c r="C22" s="5"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="13" t="s">
         <v>29</v>
       </c>
@@ -2499,7 +2762,7 @@
       <c r="C23" s="5"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="s">
         <v>29</v>
       </c>
@@ -2509,7 +2772,7 @@
       <c r="C24" s="5"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="7" t="s">
         <v>38</v>
       </c>
@@ -2519,7 +2782,7 @@
       <c r="C25" s="5"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="7" t="s">
         <v>29</v>
       </c>
@@ -2529,7 +2792,7 @@
       <c r="C26" s="5"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="7" t="s">
         <v>32</v>
       </c>
@@ -2539,7 +2802,7 @@
       <c r="C27" s="5"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
         <v>32</v>
       </c>
@@ -2549,7 +2812,7 @@
       <c r="C28" s="5"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="s">
         <v>32</v>
       </c>
@@ -2559,7 +2822,7 @@
       <c r="C29" s="5"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="12" t="s">
         <v>34</v>
       </c>
@@ -2569,7 +2832,7 @@
       <c r="C30" s="5"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="13" t="s">
         <v>34</v>
       </c>
@@ -2577,7 +2840,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="9" t="s">
         <v>47</v>
       </c>
@@ -2585,7 +2848,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="7" t="s">
         <v>34</v>
       </c>
@@ -2593,7 +2856,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="12" t="s">
         <v>36</v>
       </c>
@@ -2603,7 +2866,7 @@
       <c r="C34" s="12"/>
       <c r="D34" s="5"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="13" t="s">
         <v>36</v>
       </c>
@@ -2613,7 +2876,7 @@
       <c r="C35" s="7"/>
       <c r="D35" s="5"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="s">
         <v>53</v>
       </c>
@@ -2623,7 +2886,7 @@
       <c r="C36" s="7"/>
       <c r="D36" s="5"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="7" t="s">
         <v>36</v>
       </c>
@@ -2633,7 +2896,7 @@
       <c r="C37" s="7"/>
       <c r="D37" s="5"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="7" t="s">
         <v>39</v>
       </c>
@@ -2643,7 +2906,7 @@
       <c r="C38" s="7"/>
       <c r="D38" s="5"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="5" t="s">
         <v>39</v>
       </c>
@@ -2653,7 +2916,7 @@
       <c r="C39" s="12"/>
       <c r="D39" s="5"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="7" t="s">
         <v>40</v>
       </c>
@@ -2663,7 +2926,7 @@
       <c r="C40" s="7"/>
       <c r="D40" s="5"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A41" s="5" t="s">
         <v>40</v>
       </c>
@@ -2671,7 +2934,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A42" s="7" t="s">
         <v>41</v>
       </c>
@@ -2679,7 +2942,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A43" s="9" t="s">
         <v>41</v>
       </c>
@@ -2687,7 +2950,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A44" s="9" t="s">
         <v>41</v>
       </c>
@@ -2695,7 +2958,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A45" s="7" t="s">
         <v>42</v>
       </c>
@@ -2703,7 +2966,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A46" s="5" t="s">
         <v>42</v>
       </c>
@@ -2711,7 +2974,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A47" s="12" t="s">
         <v>44</v>
       </c>
@@ -2719,7 +2982,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A48" s="13" t="s">
         <v>44</v>
       </c>
@@ -2727,7 +2990,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="9" t="s">
         <v>68</v>
       </c>
@@ -2735,7 +2998,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="7" t="s">
         <v>68</v>
       </c>
@@ -2743,7 +3006,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="7" t="s">
         <v>68</v>
       </c>
@@ -2751,7 +3014,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="7" t="s">
         <v>48</v>
       </c>
@@ -2759,7 +3022,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="5" t="s">
         <v>48</v>
       </c>
@@ -2767,7 +3030,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="12" t="s">
         <v>49</v>
       </c>
@@ -2775,7 +3038,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="13" t="s">
         <v>49</v>
       </c>
@@ -2783,7 +3046,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="9" t="s">
         <v>73</v>
       </c>
@@ -2791,7 +3054,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="7" t="s">
         <v>73</v>
       </c>
@@ -2799,7 +3062,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="7" t="s">
         <v>73</v>
       </c>
@@ -2807,7 +3070,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="7" t="s">
         <v>52</v>
       </c>
@@ -2815,7 +3078,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="9" t="s">
         <v>52</v>
       </c>
@@ -2823,7 +3086,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="9" t="s">
         <v>52</v>
       </c>
@@ -2831,7 +3094,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="7" t="s">
         <v>52</v>
       </c>
@@ -2839,7 +3102,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="5" t="s">
         <v>54</v>
       </c>
@@ -2847,7 +3110,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="9" t="s">
         <v>55</v>
       </c>
@@ -2855,7 +3118,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A65" s="9" t="s">
         <v>55</v>
       </c>
@@ -2863,7 +3126,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="13" t="s">
         <v>56</v>
       </c>
@@ -2871,7 +3134,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="9" t="s">
         <v>56</v>
       </c>
@@ -2879,7 +3142,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="9" t="s">
         <v>59</v>
       </c>
@@ -2887,7 +3150,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="9" t="s">
         <v>74</v>
       </c>
@@ -2895,7 +3158,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="7" t="s">
         <v>59</v>
       </c>
@@ -2903,7 +3166,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="7" t="s">
         <v>59</v>
       </c>
@@ -2911,7 +3174,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="9" t="s">
         <v>61</v>
       </c>
@@ -2919,7 +3182,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="9" t="s">
         <v>61</v>
       </c>
@@ -2927,7 +3190,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="9" t="s">
         <v>62</v>
       </c>
@@ -2935,7 +3198,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="9" t="s">
         <v>62</v>
       </c>
@@ -2943,7 +3206,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="5" t="s">
         <v>64</v>
       </c>
@@ -2951,7 +3214,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="9" t="s">
         <v>67</v>
       </c>
@@ -2959,7 +3222,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A78" s="9" t="s">
         <v>75</v>
       </c>
@@ -2967,7 +3230,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A79" s="7" t="s">
         <v>67</v>
       </c>
@@ -2975,7 +3238,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A80" s="13" t="s">
         <v>69</v>
       </c>
@@ -2983,7 +3246,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="9" t="s">
         <v>69</v>
       </c>
@@ -2991,7 +3254,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A82" s="7" t="s">
         <v>69</v>
       </c>
@@ -2999,7 +3262,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A83" s="7" t="s">
         <v>69</v>
       </c>
@@ -3007,7 +3270,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A84" s="9" t="s">
         <v>72</v>
       </c>
@@ -3015,7 +3278,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A85" s="9" t="s">
         <v>72</v>
       </c>
@@ -3023,7 +3286,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A86" s="7" t="s">
         <v>76</v>
       </c>
@@ -3031,7 +3294,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A87" s="7" t="s">
         <v>72</v>
       </c>
@@ -3039,7 +3302,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A88" s="7" t="s">
         <v>77</v>
       </c>
@@ -3048,6 +3311,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>